<commit_message>
added etudiant import service
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerEtudiants.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerEtudiants.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mini projets\GestionDesAbsencesMigration\GestionDesAbsencesMigration\Excel files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90095354-6A2E-4AE5-B0D2-35FE09290609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,214 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+  <si>
+    <t>Cne</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>groupe</t>
+  </si>
+  <si>
+    <t>G1204587621</t>
+  </si>
+  <si>
+    <t>nom1</t>
+  </si>
+  <si>
+    <t>prenom1</t>
+  </si>
+  <si>
+    <t>email1@gmail.com</t>
+  </si>
+  <si>
+    <t>G1204587622</t>
+  </si>
+  <si>
+    <t>nom2</t>
+  </si>
+  <si>
+    <t>prenom2</t>
+  </si>
+  <si>
+    <t>G1204587623</t>
+  </si>
+  <si>
+    <t>nom3</t>
+  </si>
+  <si>
+    <t>prenom3</t>
+  </si>
+  <si>
+    <t>email2@gmail.com</t>
+  </si>
+  <si>
+    <t>email3@gmail.com</t>
+  </si>
+  <si>
+    <t>G1204587624</t>
+  </si>
+  <si>
+    <t>nom4</t>
+  </si>
+  <si>
+    <t>prenom4</t>
+  </si>
+  <si>
+    <t>G1204587625</t>
+  </si>
+  <si>
+    <t>nom5</t>
+  </si>
+  <si>
+    <t>prenom5</t>
+  </si>
+  <si>
+    <t>G1204587626</t>
+  </si>
+  <si>
+    <t>nom6</t>
+  </si>
+  <si>
+    <t>prenom6</t>
+  </si>
+  <si>
+    <t>G1204587627</t>
+  </si>
+  <si>
+    <t>nom7</t>
+  </si>
+  <si>
+    <t>prenom7</t>
+  </si>
+  <si>
+    <t>G1204587628</t>
+  </si>
+  <si>
+    <t>nom8</t>
+  </si>
+  <si>
+    <t>prenom8</t>
+  </si>
+  <si>
+    <t>G1204587629</t>
+  </si>
+  <si>
+    <t>nom9</t>
+  </si>
+  <si>
+    <t>prenom9</t>
+  </si>
+  <si>
+    <t>G1204587630</t>
+  </si>
+  <si>
+    <t>nom10</t>
+  </si>
+  <si>
+    <t>prenom10</t>
+  </si>
+  <si>
+    <t>G1204587631</t>
+  </si>
+  <si>
+    <t>nom11</t>
+  </si>
+  <si>
+    <t>prenom11</t>
+  </si>
+  <si>
+    <t>G1204587632</t>
+  </si>
+  <si>
+    <t>nom12</t>
+  </si>
+  <si>
+    <t>prenom12</t>
+  </si>
+  <si>
+    <t>G1204587633</t>
+  </si>
+  <si>
+    <t>nom13</t>
+  </si>
+  <si>
+    <t>prenom13</t>
+  </si>
+  <si>
+    <t>G1204587634</t>
+  </si>
+  <si>
+    <t>nom14</t>
+  </si>
+  <si>
+    <t>prenom14</t>
+  </si>
+  <si>
+    <t>email4@gmail.com</t>
+  </si>
+  <si>
+    <t>email5@gmail.com</t>
+  </si>
+  <si>
+    <t>email6@gmail.com</t>
+  </si>
+  <si>
+    <t>email7@gmail.com</t>
+  </si>
+  <si>
+    <t>email8@gmail.com</t>
+  </si>
+  <si>
+    <t>email9@gmail.com</t>
+  </si>
+  <si>
+    <t>email10@gmail.com</t>
+  </si>
+  <si>
+    <t>email11@gmail.com</t>
+  </si>
+  <si>
+    <t>email12@gmail.com</t>
+  </si>
+  <si>
+    <t>email13@gmail.com</t>
+  </si>
+  <si>
+    <t>email14@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +254,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +541,294 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E6:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{6460B8E7-35C3-4ADD-A135-B90DDFB7DF61}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{1C527680-F2F0-4228-A62C-A6ACBB4041C9}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{905B8E94-D5F7-45E3-BEB9-E9A0BE6B939B}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{69B4AF62-BF2F-40CD-891F-AF8B6D2F7E23}"/>
+    <hyperlink ref="H13" r:id="rId5" xr:uid="{40F89FCA-A549-466C-9D62-5565A862DD9A}"/>
+    <hyperlink ref="H16" r:id="rId6" xr:uid="{80D34A5A-E97C-412F-A67B-ED2E192BCF75}"/>
+    <hyperlink ref="H19" r:id="rId7" xr:uid="{A6CE5300-D157-448E-A7F7-6DFAD92E70C4}"/>
+    <hyperlink ref="H11" r:id="rId8" xr:uid="{4F1FC7F1-55DD-455D-B3B5-97DCE990BC81}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{72328D15-012B-4EB0-A136-3A03EF28D6B1}"/>
+    <hyperlink ref="H17" r:id="rId10" xr:uid="{32EED1AE-9014-4AA6-917C-BC6DF2AEF64A}"/>
+    <hyperlink ref="H20" r:id="rId11" xr:uid="{17525905-A4BD-4507-B0C8-4322144BBCD5}"/>
+    <hyperlink ref="H12" r:id="rId12" xr:uid="{2DC5F91F-E864-491C-965A-59BA8CA87B26}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{2832DA9F-CBA8-43C7-B6F2-AA9CDF1AD0C8}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{2AF75412-C078-4E33-BA34-40F825D48B0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>